<commit_message>
jo/update working example full
</commit_message>
<xml_diff>
--- a/config/optimization_engine/config_optimization/InitialValues.xlsx
+++ b/config/optimization_engine/config_optimization/InitialValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="7905" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="8505" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>tag</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Y1</t>
-  </si>
-  <si>
-    <t>Z1</t>
   </si>
   <si>
     <t>X2</t>
@@ -418,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +436,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -496,10 +493,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>200</v>
@@ -513,15 +510,15 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -538,15 +535,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -557,12 +551,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -573,18 +570,18 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -606,17 +603,6 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
jo/update finish first iteration of the codes
</commit_message>
<xml_diff>
--- a/config/optimization_engine/config_optimization/InitialValues.xlsx
+++ b/config/optimization_engine/config_optimization/InitialValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="8505" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="9105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>tag</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>init_values</t>
+  </si>
+  <si>
+    <t>Z1</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,21 +507,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -526,70 +526,70 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
-        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>500</v>
@@ -597,12 +597,23 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>500</v>
       </c>
     </row>

</xml_diff>